<commit_message>
Payment Subject added to SKU
</commit_message>
<xml_diff>
--- a/data/FOR_KAS/TODO.xlsx
+++ b/data/FOR_KAS/TODO.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="309">
   <si>
     <t>ALTER PROCEDURE APPENDPILOT(</t>
   </si>
@@ -890,18 +890,12 @@
     <t>На вход</t>
   </si>
   <si>
-    <t>с секции cm код валюты нал/безнал будет работать? Нечем тестить</t>
-  </si>
-  <si>
     <t>в секции ct  строка отдел должен быть 4, и чтоб можно было выбирать склад при продаже, тогда 1</t>
   </si>
   <si>
     <t>см скан в форматах, там подробнее</t>
   </si>
   <si>
-    <t>нумерация сквозная должна быть по хорошему, иначе в Домине ченить при акцепте отрыгнет запросто</t>
-  </si>
-  <si>
     <t>поле Фронтол</t>
   </si>
   <si>
@@ -978,6 +972,18 @@
   </si>
   <si>
     <t>попробовать вообще снать кассу, всосет ее?</t>
+  </si>
+  <si>
+    <t>Номера чеков в кассовой ленте идут сквозняком, на день не сбрасваются, это фича?</t>
+  </si>
+  <si>
+    <t>нумерация лент сквозная должна быть по хорошему, иначе в Домине ченить при акцепте отрыгнет запросто</t>
+  </si>
+  <si>
+    <t>Это можно удадить из домино</t>
+  </si>
+  <si>
+    <t>с секции cm код валюты нал/безнал будет работать? Нечем тестить вбираю карту, не работает, и не будет, это  ж код валют, в атолловском 7 тип вместо безнала мож поэтому</t>
   </si>
 </sst>
 </file>
@@ -1381,7 +1387,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1389,10 +1395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1402,7 +1408,7 @@
     <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="45" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="221.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1410,13 +1416,13 @@
         <v>265</v>
       </c>
       <c r="B1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C1" t="s">
         <v>228</v>
       </c>
       <c r="D1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E1" t="s">
         <v>236</v>
@@ -1430,7 +1436,7 @@
         <v>274</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E2" t="s">
         <v>234</v>
@@ -1444,13 +1450,13 @@
         <v>274</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E3" t="s">
         <v>234</v>
       </c>
       <c r="F3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1478,7 +1484,7 @@
         <v>231</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1492,10 +1498,10 @@
         <v>231</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1509,10 +1515,10 @@
         <v>231</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1526,7 +1532,7 @@
         <v>231</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1546,7 +1552,7 @@
         <v>234</v>
       </c>
       <c r="F9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1560,7 +1566,7 @@
         <v>238</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E10" t="s">
         <v>239</v>
@@ -1580,13 +1586,13 @@
         <v>257</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E11" t="s">
         <v>239</v>
       </c>
       <c r="F11" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1600,7 +1606,7 @@
         <v>257</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E12" t="s">
         <v>239</v>
@@ -1620,7 +1626,7 @@
         <v>257</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E13" t="s">
         <v>235</v>
@@ -1640,13 +1646,13 @@
         <v>251</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E14" t="s">
         <v>239</v>
       </c>
       <c r="F14" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1660,7 +1666,7 @@
         <v>264</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E15" t="s">
         <v>239</v>
@@ -1677,16 +1683,16 @@
         <v>266</v>
       </c>
       <c r="C16" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E16" t="s">
         <v>235</v>
       </c>
       <c r="F16" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1700,13 +1706,13 @@
         <v>263</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E17" t="s">
         <v>234</v>
       </c>
       <c r="F17" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1724,7 +1730,7 @@
         <v>234</v>
       </c>
       <c r="F18" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1738,7 +1744,7 @@
         <v>263</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E19" t="s">
         <v>234</v>
@@ -1758,13 +1764,13 @@
         <v>242</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E20" t="s">
         <v>235</v>
       </c>
       <c r="F20" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1784,7 +1790,7 @@
         <v>239</v>
       </c>
       <c r="F21" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1792,34 +1798,40 @@
         <v>276</v>
       </c>
       <c r="F24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="D25" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F25" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="D26" s="4" t="s">
-        <v>256</v>
+      <c r="D26" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="E26" t="s">
+        <v>235</v>
       </c>
       <c r="F26" t="s">
-        <v>277</v>
+        <v>308</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="D27" s="4" t="s">
-        <v>256</v>
+      <c r="B27" t="s">
+        <v>307</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>255</v>
       </c>
       <c r="E27" t="s">
         <v>235</v>
       </c>
       <c r="F27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1827,114 +1839,125 @@
         <v>256</v>
       </c>
       <c r="F28" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="D29" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F29" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="C31" s="7" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="7" customFormat="1">
+      <c r="D30" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="7" customFormat="1"/>
+    <row r="32" spans="1:6" s="7" customFormat="1"/>
+    <row r="33" spans="1:6" s="7" customFormat="1"/>
+    <row r="34" spans="1:6">
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="C35" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="D31" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D35" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="E35" t="s">
         <v>235</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F35" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
-        <v>282</v>
-      </c>
-      <c r="D32" s="2" t="s">
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>280</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="E32" t="s">
-        <v>235</v>
-      </c>
-      <c r="F32" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" t="s">
-        <v>282</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="E35" t="s">
-        <v>234</v>
-      </c>
-      <c r="F35" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="D36" s="4" t="s">
-        <v>256</v>
       </c>
       <c r="E36" t="s">
         <v>235</v>
       </c>
       <c r="F36" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>280</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="E39" t="s">
+        <v>234</v>
+      </c>
+      <c r="F39" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="D40" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E40" t="s">
+        <v>235</v>
+      </c>
+      <c r="F40" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="D41" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E41" t="s">
+        <v>298</v>
+      </c>
+      <c r="F41" t="s">
         <v>299</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="D37" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="E37" t="s">
-        <v>300</v>
-      </c>
-      <c r="F37" t="s">
-        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BMODE logic changed to type 11 all marked is textile
</commit_message>
<xml_diff>
--- a/data/FOR_KAS/TODO.xlsx
+++ b/data/FOR_KAS/TODO.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Итоги" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Лист1" sheetId="2" r:id="rId3"/>
+    <sheet name="Чипы" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="319">
   <si>
     <t>ALTER PROCEDURE APPENDPILOT(</t>
   </si>
@@ -944,9 +945,6 @@
     <t>Приоритет формат атол</t>
   </si>
   <si>
-    <t>В настройках обмена имена файлов должны быть явно указаны *.txt для забираемых и  in.f для флага</t>
-  </si>
-  <si>
     <t>Кастомное поле, не влияет теперь</t>
   </si>
   <si>
@@ -962,9 +960,6 @@
     <t>В домино код цены? Зачем оно?</t>
   </si>
   <si>
-    <t xml:space="preserve">BMODE=3 не маркированный BMODE=7 есть марка ЧЗ </t>
-  </si>
-  <si>
     <t>Социальная цена, не влияет, можно вырезать</t>
   </si>
   <si>
@@ -980,10 +975,46 @@
     <t>нумерация лент сквозная должна быть по хорошему, иначе в Домине ченить при акцепте отрыгнет запросто</t>
   </si>
   <si>
-    <t>Это можно удадить из домино</t>
-  </si>
-  <si>
     <t>с секции cm код валюты нал/безнал будет работать? Нечем тестить вбираю карту, не работает, и не будет, это  ж код валют, в атолловском 7 тип вместо безнала мож поэтому</t>
+  </si>
+  <si>
+    <t>Номера дисконтных карт обрезаются до 8 знаков сначала</t>
+  </si>
+  <si>
+    <t>Это можно удалить из домино</t>
+  </si>
+  <si>
+    <t>В настройках обмена имена файлов должны быть явно указаны *.txt для забираемых и файл флага</t>
+  </si>
+  <si>
+    <t>BMODE=3 не маркированный BMODE=7 есть марка ЧЗ   !!!Это так не работает, нужно тип товара явно указывать</t>
+  </si>
+  <si>
+    <t>4680096523469</t>
+  </si>
+  <si>
+    <t>Полотенце</t>
+  </si>
+  <si>
+    <t>Одеколон</t>
+  </si>
+  <si>
+    <t>4603023445153</t>
+  </si>
+  <si>
+    <t>Обувь</t>
+  </si>
+  <si>
+    <t>4610088860272</t>
+  </si>
+  <si>
+    <t>0104680096523469215K("CpqVU=!2m91EE0992Rk9MnWQmteMsiYrrVWQSVt1KtRJ/BCPEx2AVFiNSTE4=</t>
+  </si>
+  <si>
+    <t>0104603023445153215!mz+ICGow/&amp;l91EE1092ZQm0bhd5FNZMPiIVFAlSOsOx9Z+N+GlijtMyoPFn4M8=</t>
+  </si>
+  <si>
+    <t>0104610088860272215,WCxpvXdWyf39100C292+kL2Zgd9b4EK0C9B/3PmEyWt1Ai2rv4/hN7lbt0dirCH586t2WgSyCxdLGQEmt7hlRZs5Ohu2yxeGBZQmO43hg==</t>
   </si>
 </sst>
 </file>
@@ -1096,7 +1127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1115,6 +1146,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1397,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1592,7 +1625,7 @@
         <v>239</v>
       </c>
       <c r="F11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1652,7 +1685,7 @@
         <v>239</v>
       </c>
       <c r="F14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1692,7 +1725,7 @@
         <v>235</v>
       </c>
       <c r="F16" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1705,14 +1738,14 @@
       <c r="C17" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>284</v>
+      <c r="D17" s="6" t="s">
+        <v>255</v>
       </c>
       <c r="E17" t="s">
         <v>234</v>
       </c>
       <c r="F17" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1770,7 +1803,7 @@
         <v>235</v>
       </c>
       <c r="F20" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1783,8 +1816,8 @@
       <c r="C21" t="s">
         <v>269</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>249</v>
+      <c r="D21" s="13" t="s">
+        <v>284</v>
       </c>
       <c r="E21" t="s">
         <v>239</v>
@@ -1817,7 +1850,7 @@
         <v>235</v>
       </c>
       <c r="F26" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1839,7 +1872,7 @@
         <v>256</v>
       </c>
       <c r="F28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1847,7 +1880,7 @@
         <v>284</v>
       </c>
       <c r="F29" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="7" customFormat="1">
@@ -1855,10 +1888,17 @@
         <v>256</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="7" customFormat="1"/>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="7" customFormat="1">
+      <c r="D31" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>306</v>
+      </c>
+    </row>
     <row r="32" spans="1:6" s="7" customFormat="1"/>
     <row r="33" spans="1:6" s="7" customFormat="1"/>
     <row r="34" spans="1:6">
@@ -1935,7 +1975,7 @@
         <v>234</v>
       </c>
       <c r="F39" t="s">
-        <v>295</v>
+        <v>308</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1946,7 +1986,7 @@
         <v>235</v>
       </c>
       <c r="F40" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1954,10 +1994,10 @@
         <v>249</v>
       </c>
       <c r="E41" t="s">
+        <v>297</v>
+      </c>
+      <c r="F41" t="s">
         <v>298</v>
-      </c>
-      <c r="F41" t="s">
-        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -3436,4 +3476,89 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="14"/>
+    <col min="2" max="2" width="14.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="146.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="D1" s="15">
+        <f t="shared" ref="D1:D3" si="0">LEN(C1)</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D2" s="15">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="D3" s="15">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="D4" s="15"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="C8" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="C9" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="C10" s="15" t="b">
+        <f>EXACT(C8,C9)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>